<commit_message>
Added metabolite object and csv writer
</commit_message>
<xml_diff>
--- a/data/KnowledgeBase.xlsx
+++ b/data/KnowledgeBase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolites" sheetId="4" r:id="rId1"/>
@@ -20937,12 +20937,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M724"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AI723" sqref="AI723"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R8" sqref="R8"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -44185,12 +44185,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K527"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AN526" sqref="AN526"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>